<commit_message>
Notebooks cleaned and updated as needed.
</commit_message>
<xml_diff>
--- a/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
+++ b/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
@@ -2280,7 +2280,7 @@
       </c>
       <c r="B2" s="125" t="inlineStr">
         <is>
-          <t>01/13/22</t>
+          <t>08/10/23</t>
         </is>
       </c>
       <c r="C2" s="126" t="n"/>
@@ -2885,45 +2885,45 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E15:I15"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="G9:I9"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B15:B16">
     <cfRule type="cellIs" priority="15" operator="equal" dxfId="0">
@@ -2962,36 +2962,36 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="13">
-    <dataValidation sqref="B24" showErrorMessage="1" showInputMessage="1" allowBlank="1" promptTitle="Pool Name:" prompt="Must match label on tube"/>
-    <dataValidation sqref="B17" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="0%-25%" type="decimal">
+    <dataValidation sqref="B24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" promptTitle="Pool Name:" prompt="Must match label on tube"/>
+    <dataValidation sqref="B17" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="0%-25%" type="decimal">
       <formula1>0</formula1>
       <formula2>25</formula2>
     </dataValidation>
-    <dataValidation sqref="F24 H24:I24" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Write the actual sequence in.  NOT the Index number code."/>
-    <dataValidation sqref="B15:B16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="F24 H24:I24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Write the actual sequence in.  NOT the Index number code."/>
+    <dataValidation sqref="B15:B16" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation sqref="B21" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Single or Dual" type="list">
+    <dataValidation sqref="B21" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Single or Dual" type="list">
       <formula1>"Single, Dual"</formula1>
     </dataValidation>
-    <dataValidation sqref="B8:C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Moores Cancer Center" type="list">
+    <dataValidation sqref="B8:C8" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Moores Cancer Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="B9:C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Diabetes Research Center" type="list">
+    <dataValidation sqref="B9:C9" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Diabetes Research Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="A24" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Sequencing files will be returned with this name.  Please see instructions for restrictions on sample naming."/>
-    <dataValidation sqref="B19:C19" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="A24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Sequencing files will be returned with this name.  Please see instructions for restrictions on sample naming."/>
+    <dataValidation sqref="B19:C19" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"SR75,SR100,PE50,PE10X ATAC,PE10X ATAC Multiome,PE75,PE100,PE10x RNA,PE150,PE250,PE300,Other (Specify in Comments)"</formula1>
     </dataValidation>
-    <dataValidation sqref="B18:C18" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="B18:C18" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"MiSeq, MiSeq Nano, MiSeq Micro, HiSeq4000,NovaSeq SP,NovaSeq S1,NovaSeq S2,NovaSeq S4,Other (specify in comments)"</formula1>
     </dataValidation>
-    <dataValidation sqref="A20" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?"/>
-    <dataValidation sqref="B20:C20" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?" type="list">
+    <dataValidation sqref="A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?"/>
+    <dataValidation sqref="B20:C20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?" type="list">
       <formula1>"No-Standard Illumina Primers are fine, Yes but mix with Illumina Seq Primers, Yes ONLY Custom Primer Required"</formula1>
     </dataValidation>
-    <dataValidation sqref="B10:C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="GI Center" type="list">
+    <dataValidation sqref="B10:C10" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="GI Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3237,20 +3237,20 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A3:F3"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A4:F4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation sqref="L14:L65526" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="L14:L65526" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"nanodrop, qubit"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Reviewed and cleared notebooks as needed.
</commit_message>
<xml_diff>
--- a/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
+++ b/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
@@ -2280,7 +2280,7 @@
       </c>
       <c r="B2" s="125" t="inlineStr">
         <is>
-          <t>01/13/22</t>
+          <t>08/10/23</t>
         </is>
       </c>
       <c r="C2" s="126" t="n"/>
@@ -2885,45 +2885,45 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E15:I15"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="G9:I9"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B15:B16">
     <cfRule type="cellIs" priority="15" operator="equal" dxfId="0">
@@ -2962,36 +2962,36 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="13">
-    <dataValidation sqref="B24" showErrorMessage="1" showInputMessage="1" allowBlank="1" promptTitle="Pool Name:" prompt="Must match label on tube"/>
-    <dataValidation sqref="B17" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="0%-25%" type="decimal">
+    <dataValidation sqref="B24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" promptTitle="Pool Name:" prompt="Must match label on tube"/>
+    <dataValidation sqref="B17" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="0%-25%" type="decimal">
       <formula1>0</formula1>
       <formula2>25</formula2>
     </dataValidation>
-    <dataValidation sqref="F24 H24:I24" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Write the actual sequence in.  NOT the Index number code."/>
-    <dataValidation sqref="B15:B16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="F24 H24:I24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Write the actual sequence in.  NOT the Index number code."/>
+    <dataValidation sqref="B15:B16" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation sqref="B21" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Single or Dual" type="list">
+    <dataValidation sqref="B21" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Single or Dual" type="list">
       <formula1>"Single, Dual"</formula1>
     </dataValidation>
-    <dataValidation sqref="B8:C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Moores Cancer Center" type="list">
+    <dataValidation sqref="B8:C8" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Moores Cancer Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="B9:C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Diabetes Research Center" type="list">
+    <dataValidation sqref="B9:C9" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Diabetes Research Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="A24" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Sequencing files will be returned with this name.  Please see instructions for restrictions on sample naming."/>
-    <dataValidation sqref="B19:C19" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="A24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Sequencing files will be returned with this name.  Please see instructions for restrictions on sample naming."/>
+    <dataValidation sqref="B19:C19" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"SR75,SR100,PE50,PE10X ATAC,PE10X ATAC Multiome,PE75,PE100,PE10x RNA,PE150,PE250,PE300,Other (Specify in Comments)"</formula1>
     </dataValidation>
-    <dataValidation sqref="B18:C18" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="B18:C18" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"MiSeq, MiSeq Nano, MiSeq Micro, HiSeq4000,NovaSeq SP,NovaSeq S1,NovaSeq S2,NovaSeq S4,Other (specify in comments)"</formula1>
     </dataValidation>
-    <dataValidation sqref="A20" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?"/>
-    <dataValidation sqref="B20:C20" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?" type="list">
+    <dataValidation sqref="A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?"/>
+    <dataValidation sqref="B20:C20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?" type="list">
       <formula1>"No-Standard Illumina Primers are fine, Yes but mix with Illumina Seq Primers, Yes ONLY Custom Primer Required"</formula1>
     </dataValidation>
-    <dataValidation sqref="B10:C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="GI Center" type="list">
+    <dataValidation sqref="B10:C10" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="GI Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3237,20 +3237,20 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A3:F3"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A4:F4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation sqref="L14:L65526" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="L14:L65526" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"nanodrop, qubit"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fixes 122 v2 (#139)
* Sample_Well, well_id -> well_id_384

* Reviewed and cleared notebooks as needed.
</commit_message>
<xml_diff>
--- a/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
+++ b/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
@@ -2280,7 +2280,7 @@
       </c>
       <c r="B2" s="125" t="inlineStr">
         <is>
-          <t>01/13/22</t>
+          <t>08/10/23</t>
         </is>
       </c>
       <c r="C2" s="126" t="n"/>
@@ -2885,45 +2885,45 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E15:I15"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="G9:I9"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B15:B16">
     <cfRule type="cellIs" priority="15" operator="equal" dxfId="0">
@@ -2962,36 +2962,36 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="13">
-    <dataValidation sqref="B24" showErrorMessage="1" showInputMessage="1" allowBlank="1" promptTitle="Pool Name:" prompt="Must match label on tube"/>
-    <dataValidation sqref="B17" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="0%-25%" type="decimal">
+    <dataValidation sqref="B24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" promptTitle="Pool Name:" prompt="Must match label on tube"/>
+    <dataValidation sqref="B17" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="0%-25%" type="decimal">
       <formula1>0</formula1>
       <formula2>25</formula2>
     </dataValidation>
-    <dataValidation sqref="F24 H24:I24" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Write the actual sequence in.  NOT the Index number code."/>
-    <dataValidation sqref="B15:B16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="F24 H24:I24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Write the actual sequence in.  NOT the Index number code."/>
+    <dataValidation sqref="B15:B16" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation sqref="B21" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Single or Dual" type="list">
+    <dataValidation sqref="B21" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Single or Dual" type="list">
       <formula1>"Single, Dual"</formula1>
     </dataValidation>
-    <dataValidation sqref="B8:C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Moores Cancer Center" type="list">
+    <dataValidation sqref="B8:C8" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Moores Cancer Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="B9:C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Diabetes Research Center" type="list">
+    <dataValidation sqref="B9:C9" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Diabetes Research Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="A24" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Sequencing files will be returned with this name.  Please see instructions for restrictions on sample naming."/>
-    <dataValidation sqref="B19:C19" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="A24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Sequencing files will be returned with this name.  Please see instructions for restrictions on sample naming."/>
+    <dataValidation sqref="B19:C19" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"SR75,SR100,PE50,PE10X ATAC,PE10X ATAC Multiome,PE75,PE100,PE10x RNA,PE150,PE250,PE300,Other (Specify in Comments)"</formula1>
     </dataValidation>
-    <dataValidation sqref="B18:C18" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="B18:C18" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"MiSeq, MiSeq Nano, MiSeq Micro, HiSeq4000,NovaSeq SP,NovaSeq S1,NovaSeq S2,NovaSeq S4,Other (specify in comments)"</formula1>
     </dataValidation>
-    <dataValidation sqref="A20" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?"/>
-    <dataValidation sqref="B20:C20" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?" type="list">
+    <dataValidation sqref="A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?"/>
+    <dataValidation sqref="B20:C20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?" type="list">
       <formula1>"No-Standard Illumina Primers are fine, Yes but mix with Illumina Seq Primers, Yes ONLY Custom Primer Required"</formula1>
     </dataValidation>
-    <dataValidation sqref="B10:C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="GI Center" type="list">
+    <dataValidation sqref="B10:C10" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="GI Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3237,20 +3237,20 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A3:F3"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A4:F4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation sqref="L14:L65526" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="L14:L65526" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"nanodrop, qubit"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fix tests monday oct 23
</commit_message>
<xml_diff>
--- a/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
+++ b/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
@@ -2280,7 +2280,7 @@
       </c>
       <c r="B2" s="125" t="inlineStr">
         <is>
-          <t>10/13/23</t>
+          <t>01/13/22</t>
         </is>
       </c>
       <c r="C2" s="126" t="n"/>
@@ -2885,45 +2885,45 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G5:I5"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="B19:C19"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="E2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="E15:I15"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="B15:B16">
     <cfRule type="cellIs" priority="15" operator="equal" dxfId="0">
@@ -2962,36 +2962,36 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="13">
-    <dataValidation sqref="B24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" promptTitle="Pool Name:" prompt="Must match label on tube"/>
-    <dataValidation sqref="B17" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="0%-25%" type="decimal">
+    <dataValidation sqref="B24" showErrorMessage="1" showInputMessage="1" allowBlank="1" promptTitle="Pool Name:" prompt="Must match label on tube"/>
+    <dataValidation sqref="B17" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="0%-25%" type="decimal">
       <formula1>0</formula1>
       <formula2>25</formula2>
     </dataValidation>
-    <dataValidation sqref="F24 H24:I24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Write the actual sequence in.  NOT the Index number code."/>
-    <dataValidation sqref="B15:B16" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="F24 H24:I24" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Write the actual sequence in.  NOT the Index number code."/>
+    <dataValidation sqref="B15:B16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation sqref="B21" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Single or Dual" type="list">
+    <dataValidation sqref="B21" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Single or Dual" type="list">
       <formula1>"Single, Dual"</formula1>
     </dataValidation>
-    <dataValidation sqref="B8:C8" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Moores Cancer Center" type="list">
+    <dataValidation sqref="B8:C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Moores Cancer Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="B9:C9" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Diabetes Research Center" type="list">
+    <dataValidation sqref="B9:C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Diabetes Research Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="A24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Sequencing files will be returned with this name.  Please see instructions for restrictions on sample naming."/>
-    <dataValidation sqref="B19:C19" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="A24" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Sequencing files will be returned with this name.  Please see instructions for restrictions on sample naming."/>
+    <dataValidation sqref="B19:C19" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"SR75,SR100,PE50,PE10X ATAC,PE10X ATAC Multiome,PE75,PE100,PE10x RNA,PE150,PE250,PE300,Other (Specify in Comments)"</formula1>
     </dataValidation>
-    <dataValidation sqref="B18:C18" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="B18:C18" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"MiSeq, MiSeq Nano, MiSeq Micro, HiSeq4000,NovaSeq SP,NovaSeq S1,NovaSeq S2,NovaSeq S4,Other (specify in comments)"</formula1>
     </dataValidation>
-    <dataValidation sqref="A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?"/>
-    <dataValidation sqref="B20:C20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?" type="list">
+    <dataValidation sqref="A20" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?"/>
+    <dataValidation sqref="B20:C20" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?" type="list">
       <formula1>"No-Standard Illumina Primers are fine, Yes but mix with Illumina Seq Primers, Yes ONLY Custom Primer Required"</formula1>
     </dataValidation>
-    <dataValidation sqref="B10:C10" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="GI Center" type="list">
+    <dataValidation sqref="B10:C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="GI Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3237,20 +3237,20 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A3:F3"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A4:F4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation sqref="L14:L65526" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="L14:L65526" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"nanodrop, qubit"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add tests dp (#152)
* add final tests for pooling nb

* move compress_plates_exp file

* move plate map files

* fix filepath of platemaps in compression test

* move the files back

* more path errors

* more path errors 2

* fix tests monday oct 23

* flake8 changes

* revert to original version of 2 functions; comment out 2 test cases

* try 2: remove changes to functions; remove test cases

* working notebook

* flake8 fixes

* flake8 fix
</commit_message>
<xml_diff>
--- a/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
+++ b/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
@@ -2280,7 +2280,7 @@
       </c>
       <c r="B2" s="125" t="inlineStr">
         <is>
-          <t>10/13/23</t>
+          <t>01/13/22</t>
         </is>
       </c>
       <c r="C2" s="126" t="n"/>
@@ -2885,45 +2885,45 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G5:I5"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="B19:C19"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="E2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="E15:I15"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="B15:B16">
     <cfRule type="cellIs" priority="15" operator="equal" dxfId="0">
@@ -2962,36 +2962,36 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="13">
-    <dataValidation sqref="B24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" promptTitle="Pool Name:" prompt="Must match label on tube"/>
-    <dataValidation sqref="B17" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="0%-25%" type="decimal">
+    <dataValidation sqref="B24" showErrorMessage="1" showInputMessage="1" allowBlank="1" promptTitle="Pool Name:" prompt="Must match label on tube"/>
+    <dataValidation sqref="B17" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="0%-25%" type="decimal">
       <formula1>0</formula1>
       <formula2>25</formula2>
     </dataValidation>
-    <dataValidation sqref="F24 H24:I24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Write the actual sequence in.  NOT the Index number code."/>
-    <dataValidation sqref="B15:B16" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="F24 H24:I24" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Write the actual sequence in.  NOT the Index number code."/>
+    <dataValidation sqref="B15:B16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation sqref="B21" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Single or Dual" type="list">
+    <dataValidation sqref="B21" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Single or Dual" type="list">
       <formula1>"Single, Dual"</formula1>
     </dataValidation>
-    <dataValidation sqref="B8:C8" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Moores Cancer Center" type="list">
+    <dataValidation sqref="B8:C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Moores Cancer Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="B9:C9" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Diabetes Research Center" type="list">
+    <dataValidation sqref="B9:C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Diabetes Research Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="A24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Sequencing files will be returned with this name.  Please see instructions for restrictions on sample naming."/>
-    <dataValidation sqref="B19:C19" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="A24" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Sequencing files will be returned with this name.  Please see instructions for restrictions on sample naming."/>
+    <dataValidation sqref="B19:C19" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"SR75,SR100,PE50,PE10X ATAC,PE10X ATAC Multiome,PE75,PE100,PE10x RNA,PE150,PE250,PE300,Other (Specify in Comments)"</formula1>
     </dataValidation>
-    <dataValidation sqref="B18:C18" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="B18:C18" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"MiSeq, MiSeq Nano, MiSeq Micro, HiSeq4000,NovaSeq SP,NovaSeq S1,NovaSeq S2,NovaSeq S4,Other (specify in comments)"</formula1>
     </dataValidation>
-    <dataValidation sqref="A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?"/>
-    <dataValidation sqref="B20:C20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?" type="list">
+    <dataValidation sqref="A20" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?"/>
+    <dataValidation sqref="B20:C20" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?" type="list">
       <formula1>"No-Standard Illumina Primers are fine, Yes but mix with Illumina Seq Primers, Yes ONLY Custom Primer Required"</formula1>
     </dataValidation>
-    <dataValidation sqref="B10:C10" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="GI Center" type="list">
+    <dataValidation sqref="B10:C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="GI Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3237,20 +3237,20 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A3:F3"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A4:F4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation sqref="L14:L65526" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="L14:L65526" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"nanodrop, qubit"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updates to Dev branch (#161)
* Updated README.md

* Reapply Metagenomics -> Metagenomic

* Updates to notebooks

Updates to notebooks that modify/use YYYY_MM_DD_FinRisk_33-36_samplesheet.csv.
Confirmed current csv is correct in form.
Notebooks updated to use validate_sample_sheet() correctly.
validate_sample_sheet() and its helpers updated to no longer return a
sheet object.

* tests updated

* Removing obsolete notebook + files.

Removing obsolete notebook on Rodolfo's recommendation.
Removing files that are no longer mentioned in any file in this repo.

* Updating files

* Removed obsolete test
</commit_message>
<xml_diff>
--- a/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
+++ b/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
@@ -2280,7 +2280,7 @@
       </c>
       <c r="B2" s="125" t="inlineStr">
         <is>
-          <t>01/13/22</t>
+          <t>12/12/23</t>
         </is>
       </c>
       <c r="C2" s="126" t="n"/>
@@ -2885,45 +2885,45 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E15:I15"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="G9:I9"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="B15:B16">
     <cfRule type="cellIs" priority="15" operator="equal" dxfId="0">
@@ -2962,36 +2962,36 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="13">
-    <dataValidation sqref="B24" showErrorMessage="1" showInputMessage="1" allowBlank="1" promptTitle="Pool Name:" prompt="Must match label on tube"/>
-    <dataValidation sqref="B17" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="0%-25%" type="decimal">
+    <dataValidation sqref="B24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" promptTitle="Pool Name:" prompt="Must match label on tube"/>
+    <dataValidation sqref="B17" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="0%-25%" type="decimal">
       <formula1>0</formula1>
       <formula2>25</formula2>
     </dataValidation>
-    <dataValidation sqref="F24 H24:I24" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Write the actual sequence in.  NOT the Index number code."/>
-    <dataValidation sqref="B15:B16" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="F24 H24:I24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Write the actual sequence in.  NOT the Index number code."/>
+    <dataValidation sqref="B15:B16" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation sqref="B21" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Single or Dual" type="list">
+    <dataValidation sqref="B21" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Single or Dual" type="list">
       <formula1>"Single, Dual"</formula1>
     </dataValidation>
-    <dataValidation sqref="B8:C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Moores Cancer Center" type="list">
+    <dataValidation sqref="B8:C8" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Moores Cancer Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="B9:C9" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Diabetes Research Center" type="list">
+    <dataValidation sqref="B9:C9" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Diabetes Research Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="A24" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Sequencing files will be returned with this name.  Please see instructions for restrictions on sample naming."/>
-    <dataValidation sqref="B19:C19" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="A24" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Sequencing files will be returned with this name.  Please see instructions for restrictions on sample naming."/>
+    <dataValidation sqref="B19:C19" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"SR75,SR100,PE50,PE10X ATAC,PE10X ATAC Multiome,PE75,PE100,PE10x RNA,PE150,PE250,PE300,Other (Specify in Comments)"</formula1>
     </dataValidation>
-    <dataValidation sqref="B18:C18" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="B18:C18" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"MiSeq, MiSeq Nano, MiSeq Micro, HiSeq4000,NovaSeq SP,NovaSeq S1,NovaSeq S2,NovaSeq S4,Other (specify in comments)"</formula1>
     </dataValidation>
-    <dataValidation sqref="A20" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?"/>
-    <dataValidation sqref="B20:C20" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?" type="list">
+    <dataValidation sqref="A20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?"/>
+    <dataValidation sqref="B20:C20" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="Does this submission require a custom sequencing primer? If so, is it compatable with Illumina Sequening primers?" type="list">
       <formula1>"No-Standard Illumina Primers are fine, Yes but mix with Illumina Seq Primers, Yes ONLY Custom Primer Required"</formula1>
     </dataValidation>
-    <dataValidation sqref="B10:C10" showErrorMessage="1" showInputMessage="1" allowBlank="1" prompt="GI Center" type="list">
+    <dataValidation sqref="B10:C10" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" prompt="GI Center" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3237,20 +3237,20 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A3:F3"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A4:F4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation sqref="L14:L65526" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="L14:L65526" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>"nanodrop, qubit"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Remove strict option from male_sample_sheet()
As part of cleanup, removing legacy option to allow or deny any
additional columns from appearing in the spreadsheet. Tests updated
accordingly.
</commit_message>
<xml_diff>
--- a/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
+++ b/notebooks/test_output/SampleSheets/YYYY_MM_DD_PI_Sequencing_Runs_Manifest_2021.xlsx
@@ -2280,7 +2280,7 @@
       </c>
       <c r="B2" s="125" t="inlineStr">
         <is>
-          <t>12/12/23</t>
+          <t>05/03/24</t>
         </is>
       </c>
       <c r="C2" s="126" t="n"/>
@@ -2702,7 +2702,7 @@
         </is>
       </c>
       <c r="B22" s="131" t="n">
-        <v>1536</v>
+        <v>384</v>
       </c>
       <c r="C22" s="132" t="n"/>
       <c r="D22" s="14" t="n"/>

</xml_diff>